<commit_message>
Eingangsdaten Dänemark_West um Kraftwerke gekürzt
</commit_message>
<xml_diff>
--- a/Daten/beispiel_1/Eingangsdaten/Netzeinspeisungen-E001-E003-Dänemark_West.xlsx
+++ b/Daten/beispiel_1/Eingangsdaten/Netzeinspeisungen-E001-E003-Dänemark_West.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="-15" windowWidth="14445" windowHeight="12795" activeTab="1"/>
+    <workbookView xWindow="14400" yWindow="-15" windowWidth="14445" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Kraftwerkszuordnung" sheetId="3" r:id="rId1"/>
@@ -19,14 +19,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ergebnis KEP'!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Importtabelle E001'!$A$2:$G$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Importtabelle E003'!$A$2:$G$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Kraftwerkszuordnung!$A$1:$K$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Kraftwerkszuordnung!$A$1:$K$37</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="144">
   <si>
     <t>Kraftwerk</t>
   </si>
@@ -469,8 +469,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,7 +651,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -725,6 +725,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -759,6 +760,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -934,15 +936,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -956,7 +958,7 @@
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -992,7 +994,7 @@
       </c>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>101</v>
       </c>
@@ -1036,12 +1038,12 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>1</v>
@@ -1050,25 +1052,25 @@
         <v>150</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
+        <v>0.9</v>
       </c>
       <c r="H3" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
+        <v>0</v>
       </c>
       <c r="J3" s="8">
-        <v>408.15</v>
+        <v>16.75</v>
       </c>
       <c r="K3" s="1">
         <f>IF(F3=Kraftwerkspark!$B$2,J3*Kraftwerkspark!$H$2/100,
@@ -1077,42 +1079,42 @@
 IF(F3=Kraftwerkspark!$B$5,J3*Kraftwerkspark!$H$5/100,
 IF(F3=Kraftwerkspark!$B$6,J3*Kraftwerkspark!$H$6/100,
 IF(F3=Kraftwerkspark!$B$8,J3*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>122.44499999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="17">
-        <v>380</v>
+        <v>150</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.35</v>
+        <v>0.52</v>
       </c>
       <c r="H4" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.27</v>
+        <v>0.2</v>
       </c>
       <c r="I4" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
         <v>7.125</v>
       </c>
       <c r="J4" s="8">
-        <v>1055.1500000000001</v>
+        <v>58.15</v>
       </c>
       <c r="K4" s="1">
         <f>IF(F4=Kraftwerkspark!$B$2,J4*Kraftwerkspark!$H$2/100,
@@ -1121,42 +1123,42 @@
 IF(F4=Kraftwerkspark!$B$5,J4*Kraftwerkspark!$H$5/100,
 IF(F4=Kraftwerkspark!$B$6,J4*Kraftwerkspark!$H$6/100,
 IF(F4=Kraftwerkspark!$B$8,J4*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>211.03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="17">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.9</v>
+        <v>0.42</v>
       </c>
       <c r="H5" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I5" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>0</v>
+        <v>2.85</v>
       </c>
       <c r="J5" s="8">
-        <v>16.75</v>
+        <v>623.15</v>
       </c>
       <c r="K5" s="1">
         <f>IF(F5=Kraftwerkspark!$B$2,J5*Kraftwerkspark!$H$2/100,
@@ -1165,42 +1167,42 @@
 IF(F5=Kraftwerkspark!$B$5,J5*Kraftwerkspark!$H$5/100,
 IF(F5=Kraftwerkspark!$B$6,J5*Kraftwerkspark!$H$6/100,
 IF(F5=Kraftwerkspark!$B$8,J5*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>186.94499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="17">
-        <v>380</v>
+        <v>150</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
+        <v>0.42</v>
       </c>
       <c r="H6" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I6" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
+        <v>2.85</v>
       </c>
       <c r="J6" s="8">
-        <v>808.15</v>
+        <v>376.15</v>
       </c>
       <c r="K6" s="1">
         <f>IF(F6=Kraftwerkspark!$B$2,J6*Kraftwerkspark!$H$2/100,
@@ -1209,42 +1211,42 @@
 IF(F6=Kraftwerkspark!$B$5,J6*Kraftwerkspark!$H$5/100,
 IF(F6=Kraftwerkspark!$B$6,J6*Kraftwerkspark!$H$6/100,
 IF(F6=Kraftwerkspark!$B$8,J6*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>161.63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>112.845</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="17">
-        <v>150</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>46</v>
+        <v>380</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
+        <v>0.42</v>
       </c>
       <c r="H7" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I7" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
+        <v>2.85</v>
       </c>
       <c r="J7" s="8">
-        <v>75.150000000000006</v>
+        <v>673.15</v>
       </c>
       <c r="K7" s="1">
         <f>IF(F7=Kraftwerkspark!$B$2,J7*Kraftwerkspark!$H$2/100,
@@ -1253,15 +1255,15 @@
 IF(F7=Kraftwerkspark!$B$5,J7*Kraftwerkspark!$H$5/100,
 IF(F7=Kraftwerkspark!$B$6,J7*Kraftwerkspark!$H$6/100,
 IF(F7=Kraftwerkspark!$B$8,J7*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>15.03</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>201.94499999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>1</v>
@@ -1270,25 +1272,25 @@
         <v>150</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="G8" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H8" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="I8" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
+        <v>0</v>
       </c>
       <c r="J8" s="8">
-        <v>58.15</v>
+        <v>33.15</v>
       </c>
       <c r="K8" s="1">
         <f>IF(F8=Kraftwerkspark!$B$2,J8*Kraftwerkspark!$H$2/100,
@@ -1297,42 +1299,42 @@
 IF(F8=Kraftwerkspark!$B$5,J8*Kraftwerkspark!$H$5/100,
 IF(F8=Kraftwerkspark!$B$6,J8*Kraftwerkspark!$H$6/100,
 IF(F8=Kraftwerkspark!$B$8,J8*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>11.63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="17">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
+        <v>0.52</v>
       </c>
       <c r="H9" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I9" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
+        <v>7.125</v>
       </c>
       <c r="J9" s="8">
-        <v>623.15</v>
+        <v>87.15</v>
       </c>
       <c r="K9" s="1">
         <f>IF(F9=Kraftwerkspark!$B$2,J9*Kraftwerkspark!$H$2/100,
@@ -1341,15 +1343,15 @@
 IF(F9=Kraftwerkspark!$B$5,J9*Kraftwerkspark!$H$5/100,
 IF(F9=Kraftwerkspark!$B$6,J9*Kraftwerkspark!$H$6/100,
 IF(F9=Kraftwerkspark!$B$8,J9*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>186.94499999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>17.43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>1</v>
@@ -1358,25 +1360,25 @@
         <v>150</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
+        <v>0.52</v>
       </c>
       <c r="H10" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I10" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
+        <v>7.125</v>
       </c>
       <c r="J10" s="8">
-        <v>376.15</v>
+        <v>13.85</v>
       </c>
       <c r="K10" s="1">
         <f>IF(F10=Kraftwerkspark!$B$2,J10*Kraftwerkspark!$H$2/100,
@@ -1385,42 +1387,42 @@
 IF(F10=Kraftwerkspark!$B$5,J10*Kraftwerkspark!$H$5/100,
 IF(F10=Kraftwerkspark!$B$6,J10*Kraftwerkspark!$H$6/100,
 IF(F10=Kraftwerkspark!$B$8,J10*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>112.845</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="17">
-        <v>380</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>150</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="G11" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H11" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="I11" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
+        <v>0</v>
       </c>
       <c r="J11" s="8">
-        <v>673.15</v>
+        <v>1.25</v>
       </c>
       <c r="K11" s="1">
         <f>IF(F11=Kraftwerkspark!$B$2,J11*Kraftwerkspark!$H$2/100,
@@ -1429,42 +1431,42 @@
 IF(F11=Kraftwerkspark!$B$5,J11*Kraftwerkspark!$H$5/100,
 IF(F11=Kraftwerkspark!$B$6,J11*Kraftwerkspark!$H$6/100,
 IF(F11=Kraftwerkspark!$B$8,J11*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>201.94499999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="17">
-        <v>380</v>
+        <v>150</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G12" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
+        <v>0.42</v>
       </c>
       <c r="H12" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I12" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
+        <v>2.85</v>
       </c>
       <c r="J12" s="8">
-        <v>36.15</v>
+        <v>50.15</v>
       </c>
       <c r="K12" s="1">
         <f>IF(F12=Kraftwerkspark!$B$2,J12*Kraftwerkspark!$H$2/100,
@@ -1473,24 +1475,24 @@
 IF(F12=Kraftwerkspark!$B$5,J12*Kraftwerkspark!$H$5/100,
 IF(F12=Kraftwerkspark!$B$6,J12*Kraftwerkspark!$H$6/100,
 IF(F12=Kraftwerkspark!$B$8,J12*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>7.23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>15.045</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="17">
-        <v>380</v>
+        <v>150</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>3</v>
@@ -1508,7 +1510,7 @@
         <v>7.125</v>
       </c>
       <c r="J13" s="8">
-        <v>131.15</v>
+        <v>3.15</v>
       </c>
       <c r="K13" s="1">
         <f>IF(F13=Kraftwerkspark!$B$2,J13*Kraftwerkspark!$H$2/100,
@@ -1517,42 +1519,42 @@
 IF(F13=Kraftwerkspark!$B$5,J13*Kraftwerkspark!$H$5/100,
 IF(F13=Kraftwerkspark!$B$6,J13*Kraftwerkspark!$H$6/100,
 IF(F13=Kraftwerkspark!$B$8,J13*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>26.23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="17">
-        <v>150</v>
+        <v>380</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G14" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.9</v>
+        <v>0.42</v>
       </c>
       <c r="H14" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I14" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>0</v>
+        <v>2.85</v>
       </c>
       <c r="J14" s="8">
-        <v>3.15</v>
+        <v>658.15</v>
       </c>
       <c r="K14" s="1">
         <f>IF(F14=Kraftwerkspark!$B$2,J14*Kraftwerkspark!$H$2/100,
@@ -1561,42 +1563,42 @@
 IF(F14=Kraftwerkspark!$B$5,J14*Kraftwerkspark!$H$5/100,
 IF(F14=Kraftwerkspark!$B$6,J14*Kraftwerkspark!$H$6/100,
 IF(F14=Kraftwerkspark!$B$8,J14*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>197.44499999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="17">
-        <v>150</v>
+        <v>380</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="G15" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.14000000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="H15" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="I15" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>0</v>
+        <v>7.125</v>
       </c>
       <c r="J15" s="8">
-        <v>33.15</v>
+        <v>390.15</v>
       </c>
       <c r="K15" s="1">
         <f>IF(F15=Kraftwerkspark!$B$2,J15*Kraftwerkspark!$H$2/100,
@@ -1605,15 +1607,15 @@
 IF(F15=Kraftwerkspark!$B$5,J15*Kraftwerkspark!$H$5/100,
 IF(F15=Kraftwerkspark!$B$6,J15*Kraftwerkspark!$H$6/100,
 IF(F15=Kraftwerkspark!$B$8,J15*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>78.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>1</v>
@@ -1622,7 +1624,7 @@
         <v>150</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>42</v>
@@ -1640,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="8">
-        <v>9.85</v>
+        <v>26.15</v>
       </c>
       <c r="K16" s="1">
         <f>IF(F16=Kraftwerkspark!$B$2,J16*Kraftwerkspark!$H$2/100,
@@ -1652,39 +1654,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="17">
-        <v>150</v>
+        <v>380</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="G17" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
+        <v>0.35</v>
       </c>
       <c r="H17" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
       <c r="I17" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
         <v>7.125</v>
       </c>
       <c r="J17" s="8">
-        <v>87.15</v>
+        <v>698.15</v>
       </c>
       <c r="K17" s="1">
         <f>IF(F17=Kraftwerkspark!$B$2,J17*Kraftwerkspark!$H$2/100,
@@ -1693,42 +1695,42 @@
 IF(F17=Kraftwerkspark!$B$5,J17*Kraftwerkspark!$H$5/100,
 IF(F17=Kraftwerkspark!$B$6,J17*Kraftwerkspark!$H$6/100,
 IF(F17=Kraftwerkspark!$B$8,J17*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>17.43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>139.63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="17">
-        <v>380</v>
+        <v>150</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="G18" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.35</v>
+        <v>0.9</v>
       </c>
       <c r="H18" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.27</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
+        <v>0</v>
       </c>
       <c r="J18" s="8">
-        <v>674.15</v>
+        <v>0.45</v>
       </c>
       <c r="K18" s="1">
         <f>IF(F18=Kraftwerkspark!$B$2,J18*Kraftwerkspark!$H$2/100,
@@ -1737,15 +1739,15 @@
 IF(F18=Kraftwerkspark!$B$5,J18*Kraftwerkspark!$H$5/100,
 IF(F18=Kraftwerkspark!$B$6,J18*Kraftwerkspark!$H$6/100,
 IF(F18=Kraftwerkspark!$B$8,J18*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>134.83000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>1</v>
@@ -1754,7 +1756,7 @@
         <v>150</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>3</v>
@@ -1772,7 +1774,7 @@
         <v>7.125</v>
       </c>
       <c r="J19" s="8">
-        <v>13.85</v>
+        <v>10.15</v>
       </c>
       <c r="K19" s="1">
         <f>IF(F19=Kraftwerkspark!$B$2,J19*Kraftwerkspark!$H$2/100,
@@ -1781,42 +1783,42 @@
 IF(F19=Kraftwerkspark!$B$5,J19*Kraftwerkspark!$H$5/100,
 IF(F19=Kraftwerkspark!$B$6,J19*Kraftwerkspark!$H$6/100,
 IF(F19=Kraftwerkspark!$B$8,J19*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>2.77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="17">
         <v>150</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="G20" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.14000000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="H20" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="J20" s="8">
-        <v>1.25</v>
+        <v>10</v>
       </c>
       <c r="K20" s="1">
         <f>IF(F20=Kraftwerkspark!$B$2,J20*Kraftwerkspark!$H$2/100,
@@ -1828,12 +1830,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>1</v>
@@ -1842,25 +1844,25 @@
         <v>150</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G21" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
+        <v>0.52</v>
       </c>
       <c r="H21" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I21" s="1">
         <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
+        <v>7.125</v>
       </c>
       <c r="J21" s="8">
-        <v>50.15</v>
+        <v>1.75</v>
       </c>
       <c r="K21" s="1">
         <f>IF(F21=Kraftwerkspark!$B$2,J21*Kraftwerkspark!$H$2/100,
@@ -1869,15 +1871,15 @@
 IF(F21=Kraftwerkspark!$B$5,J21*Kraftwerkspark!$H$5/100,
 IF(F21=Kraftwerkspark!$B$6,J21*Kraftwerkspark!$H$6/100,
 IF(F21=Kraftwerkspark!$B$8,J21*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>15.045</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>1</v>
@@ -1886,7 +1888,7 @@
         <v>150</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>3</v>
@@ -1904,7 +1906,7 @@
         <v>7.125</v>
       </c>
       <c r="J22" s="8">
-        <v>3.15</v>
+        <v>2.85</v>
       </c>
       <c r="K22" s="1">
         <f>IF(F22=Kraftwerkspark!$B$2,J22*Kraftwerkspark!$H$2/100,
@@ -1913,898 +1915,238 @@
 IF(F22=Kraftwerkspark!$B$5,J22*Kraftwerkspark!$H$5/100,
 IF(F22=Kraftwerkspark!$B$6,J22*Kraftwerkspark!$H$6/100,
 IF(F22=Kraftwerkspark!$B$8,J22*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="17">
-        <v>380</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
-      </c>
-      <c r="H23" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
-      </c>
-      <c r="I23" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
-      </c>
-      <c r="J23" s="8">
-        <v>658.15</v>
-      </c>
-      <c r="K23" s="1">
-        <f>IF(F23=Kraftwerkspark!$B$2,J23*Kraftwerkspark!$H$2/100,
-IF(F23=Kraftwerkspark!$B$3,J23*Kraftwerkspark!$H$3/100,
-IF(F23=Kraftwerkspark!$B$4,J23*Kraftwerkspark!$H$4/100,
-IF(F23=Kraftwerkspark!$B$5,J23*Kraftwerkspark!$H$5/100,
-IF(F23=Kraftwerkspark!$B$6,J23*Kraftwerkspark!$H$6/100,
-IF(F23=Kraftwerkspark!$B$8,J23*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>197.44499999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="17">
-        <v>150</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H24" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I24" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J24" s="8">
-        <v>9.15</v>
-      </c>
-      <c r="K24" s="1">
-        <f>IF(F24=Kraftwerkspark!$B$2,J24*Kraftwerkspark!$H$2/100,
-IF(F24=Kraftwerkspark!$B$3,J24*Kraftwerkspark!$H$3/100,
-IF(F24=Kraftwerkspark!$B$4,J24*Kraftwerkspark!$H$4/100,
-IF(F24=Kraftwerkspark!$B$5,J24*Kraftwerkspark!$H$5/100,
-IF(F24=Kraftwerkspark!$B$6,J24*Kraftwerkspark!$H$6/100,
-IF(F24=Kraftwerkspark!$B$8,J24*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="17">
-        <v>380</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H25" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I25" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J25" s="8">
-        <v>390.15</v>
-      </c>
-      <c r="K25" s="1">
-        <f>IF(F25=Kraftwerkspark!$B$2,J25*Kraftwerkspark!$H$2/100,
-IF(F25=Kraftwerkspark!$B$3,J25*Kraftwerkspark!$H$3/100,
-IF(F25=Kraftwerkspark!$B$4,J25*Kraftwerkspark!$H$4/100,
-IF(F25=Kraftwerkspark!$B$5,J25*Kraftwerkspark!$H$5/100,
-IF(F25=Kraftwerkspark!$B$6,J25*Kraftwerkspark!$H$6/100,
-IF(F25=Kraftwerkspark!$B$8,J25*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>78.03</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="17">
-        <v>150</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
-      </c>
-      <c r="H26" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
-      </c>
-      <c r="I26" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
-      </c>
-      <c r="J26" s="8">
-        <v>407.15</v>
-      </c>
-      <c r="K26" s="1">
-        <f>IF(F26=Kraftwerkspark!$B$2,J26*Kraftwerkspark!$H$2/100,
-IF(F26=Kraftwerkspark!$B$3,J26*Kraftwerkspark!$H$3/100,
-IF(F26=Kraftwerkspark!$B$4,J26*Kraftwerkspark!$H$4/100,
-IF(F26=Kraftwerkspark!$B$5,J26*Kraftwerkspark!$H$5/100,
-IF(F26=Kraftwerkspark!$B$6,J26*Kraftwerkspark!$H$6/100,
-IF(F26=Kraftwerkspark!$B$8,J26*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>122.145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="17">
-        <v>150</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.9</v>
-      </c>
-      <c r="H27" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="8">
-        <v>26.15</v>
-      </c>
-      <c r="K27" s="1">
-        <f>IF(F27=Kraftwerkspark!$B$2,J27*Kraftwerkspark!$H$2/100,
-IF(F27=Kraftwerkspark!$B$3,J27*Kraftwerkspark!$H$3/100,
-IF(F27=Kraftwerkspark!$B$4,J27*Kraftwerkspark!$H$4/100,
-IF(F27=Kraftwerkspark!$B$5,J27*Kraftwerkspark!$H$5/100,
-IF(F27=Kraftwerkspark!$B$6,J27*Kraftwerkspark!$H$6/100,
-IF(F27=Kraftwerkspark!$B$8,J27*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="17">
-        <v>380</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.35</v>
-      </c>
-      <c r="H28" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.27</v>
-      </c>
-      <c r="I28" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J28" s="8">
-        <v>698.15</v>
-      </c>
-      <c r="K28" s="1">
-        <f>IF(F28=Kraftwerkspark!$B$2,J28*Kraftwerkspark!$H$2/100,
-IF(F28=Kraftwerkspark!$B$3,J28*Kraftwerkspark!$H$3/100,
-IF(F28=Kraftwerkspark!$B$4,J28*Kraftwerkspark!$H$4/100,
-IF(F28=Kraftwerkspark!$B$5,J28*Kraftwerkspark!$H$5/100,
-IF(F28=Kraftwerkspark!$B$6,J28*Kraftwerkspark!$H$6/100,
-IF(F28=Kraftwerkspark!$B$8,J28*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>139.63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="17">
-        <v>150</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.42</v>
-      </c>
-      <c r="H29" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.3</v>
-      </c>
-      <c r="I29" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>2.85</v>
-      </c>
-      <c r="J29" s="8">
-        <v>79.150000000000006</v>
-      </c>
-      <c r="K29" s="1">
-        <f>IF(F29=Kraftwerkspark!$B$2,J29*Kraftwerkspark!$H$2/100,
-IF(F29=Kraftwerkspark!$B$3,J29*Kraftwerkspark!$H$3/100,
-IF(F29=Kraftwerkspark!$B$4,J29*Kraftwerkspark!$H$4/100,
-IF(F29=Kraftwerkspark!$B$5,J29*Kraftwerkspark!$H$5/100,
-IF(F29=Kraftwerkspark!$B$6,J29*Kraftwerkspark!$H$6/100,
-IF(F29=Kraftwerkspark!$B$8,J29*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>23.745000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="17">
-        <v>150</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.9</v>
-      </c>
-      <c r="H30" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="8">
-        <v>0.45</v>
-      </c>
-      <c r="K30" s="1">
-        <f>IF(F30=Kraftwerkspark!$B$2,J30*Kraftwerkspark!$H$2/100,
-IF(F30=Kraftwerkspark!$B$3,J30*Kraftwerkspark!$H$3/100,
-IF(F30=Kraftwerkspark!$B$4,J30*Kraftwerkspark!$H$4/100,
-IF(F30=Kraftwerkspark!$B$5,J30*Kraftwerkspark!$H$5/100,
-IF(F30=Kraftwerkspark!$B$6,J30*Kraftwerkspark!$H$6/100,
-IF(F30=Kraftwerkspark!$B$8,J30*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="17">
-        <v>150</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H31" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I31" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J31" s="8">
-        <v>10.15</v>
-      </c>
-      <c r="K31" s="1">
-        <f>IF(F31=Kraftwerkspark!$B$2,J31*Kraftwerkspark!$H$2/100,
-IF(F31=Kraftwerkspark!$B$3,J31*Kraftwerkspark!$H$3/100,
-IF(F31=Kraftwerkspark!$B$4,J31*Kraftwerkspark!$H$4/100,
-IF(F31=Kraftwerkspark!$B$5,J31*Kraftwerkspark!$H$5/100,
-IF(F31=Kraftwerkspark!$B$6,J31*Kraftwerkspark!$H$6/100,
-IF(F31=Kraftwerkspark!$B$8,J31*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="17">
-        <v>150</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G32" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.85</v>
-      </c>
-      <c r="H32" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="8">
-        <v>10</v>
-      </c>
-      <c r="K32" s="1">
-        <f>IF(F32=Kraftwerkspark!$B$2,J32*Kraftwerkspark!$H$2/100,
-IF(F32=Kraftwerkspark!$B$3,J32*Kraftwerkspark!$H$3/100,
-IF(F32=Kraftwerkspark!$B$4,J32*Kraftwerkspark!$H$4/100,
-IF(F32=Kraftwerkspark!$B$5,J32*Kraftwerkspark!$H$5/100,
-IF(F32=Kraftwerkspark!$B$6,J32*Kraftwerkspark!$H$6/100,
-IF(F32=Kraftwerkspark!$B$8,J32*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="17">
-        <v>150</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H33" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I33" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J33" s="8">
-        <v>55.15</v>
-      </c>
-      <c r="K33" s="1">
-        <f>IF(F33=Kraftwerkspark!$B$2,J33*Kraftwerkspark!$H$2/100,
-IF(F33=Kraftwerkspark!$B$3,J33*Kraftwerkspark!$H$3/100,
-IF(F33=Kraftwerkspark!$B$4,J33*Kraftwerkspark!$H$4/100,
-IF(F33=Kraftwerkspark!$B$5,J33*Kraftwerkspark!$H$5/100,
-IF(F33=Kraftwerkspark!$B$6,J33*Kraftwerkspark!$H$6/100,
-IF(F33=Kraftwerkspark!$B$8,J33*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>11.03</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="17">
-        <v>150</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H34" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I34" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J34" s="8">
-        <v>1.75</v>
-      </c>
-      <c r="K34" s="1">
-        <f>IF(F34=Kraftwerkspark!$B$2,J34*Kraftwerkspark!$H$2/100,
-IF(F34=Kraftwerkspark!$B$3,J34*Kraftwerkspark!$H$3/100,
-IF(F34=Kraftwerkspark!$B$4,J34*Kraftwerkspark!$H$4/100,
-IF(F34=Kraftwerkspark!$B$5,J34*Kraftwerkspark!$H$5/100,
-IF(F34=Kraftwerkspark!$B$6,J34*Kraftwerkspark!$H$6/100,
-IF(F34=Kraftwerkspark!$B$8,J34*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="17">
-        <v>150</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H35" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I35" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J35" s="8">
-        <v>2.85</v>
-      </c>
-      <c r="K35" s="1">
-        <f>IF(F35=Kraftwerkspark!$B$2,J35*Kraftwerkspark!$H$2/100,
-IF(F35=Kraftwerkspark!$B$3,J35*Kraftwerkspark!$H$3/100,
-IF(F35=Kraftwerkspark!$B$4,J35*Kraftwerkspark!$H$4/100,
-IF(F35=Kraftwerkspark!$B$5,J35*Kraftwerkspark!$H$5/100,
-IF(F35=Kraftwerkspark!$B$6,J35*Kraftwerkspark!$H$6/100,
-IF(F35=Kraftwerkspark!$B$8,J35*Kraftwerkspark!$H$8/100,0))))))</f>
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="20">
-        <v>150</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.52</v>
-      </c>
-      <c r="H36" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I36" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>7.125</v>
-      </c>
-      <c r="J36" s="8">
-        <v>1.25</v>
-      </c>
-      <c r="K36" s="1">
-        <f>IF(F36=Kraftwerkspark!$B$2,J36*Kraftwerkspark!$H$2/100,
-IF(F36=Kraftwerkspark!$B$3,J36*Kraftwerkspark!$H$3/100,
-IF(F36=Kraftwerkspark!$B$4,J36*Kraftwerkspark!$H$4/100,
-IF(F36=Kraftwerkspark!$B$5,J36*Kraftwerkspark!$H$5/100,
-IF(F36=Kraftwerkspark!$B$6,J36*Kraftwerkspark!$H$6/100,
-IF(F36=Kraftwerkspark!$B$8,J36*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="17">
-        <v>150</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,4,FALSE)</f>
-        <v>0.9</v>
-      </c>
-      <c r="H37" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,3,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="1">
-        <f>VLOOKUP(F:F,Kraftwerkspark!$B$2:$F$8,5,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="J37" s="8">
-        <v>7.45</v>
-      </c>
-      <c r="K37" s="1">
-        <f>IF(F37=Kraftwerkspark!$B$2,J37*Kraftwerkspark!$H$2/100,
-IF(F37=Kraftwerkspark!$B$3,J37*Kraftwerkspark!$H$3/100,
-IF(F37=Kraftwerkspark!$B$4,J37*Kraftwerkspark!$H$4/100,
-IF(F37=Kraftwerkspark!$B$5,J37*Kraftwerkspark!$H$5/100,
-IF(F37=Kraftwerkspark!$B$6,J37*Kraftwerkspark!$H$6/100,
-IF(F37=Kraftwerkspark!$B$8,J37*Kraftwerkspark!$H$8/100,0))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="26"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="26"/>
+    </row>
+    <row r="27" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="26"/>
+    </row>
+    <row r="28" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26"/>
+    </row>
+    <row r="29" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="26"/>
+    </row>
+    <row r="30" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="26"/>
+    </row>
+    <row r="31" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="26"/>
+    </row>
+    <row r="32" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="26"/>
+    </row>
+    <row r="33" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="26"/>
+    </row>
+    <row r="34" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="26"/>
+    </row>
+    <row r="35" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="26"/>
+    </row>
+    <row r="36" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="26"/>
+    </row>
+    <row r="37" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="26"/>
+    </row>
+    <row r="38" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="24"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="26"/>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="4"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="26"/>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="4"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="26"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="4"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="26"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="4"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="26"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="4"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="26"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="4"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="26"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="4"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="26"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="4"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="26"/>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="4"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="26"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="4"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="26"/>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="4"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="26"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="4"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="26"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="4"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="26"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="4"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="26"/>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="4"/>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="C54" s="5"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="5"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2813,14 +2155,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -2828,7 +2170,7 @@
     <col min="7" max="7" width="17.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
@@ -2854,7 +2196,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2862,8 +2204,8 @@
         <v>3</v>
       </c>
       <c r="C2" s="15">
-        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$52,B2,Kraftwerkszuordnung!$J$2:$J$52)</f>
-        <v>1685.2000000000003</v>
+        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$37,B2,Kraftwerkszuordnung!$J$2:$J$37)</f>
+        <v>569.04999999999995</v>
       </c>
       <c r="D2" s="3">
         <v>0.2</v>
@@ -2882,7 +2224,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2890,7 +2232,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="15">
-        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$52,B3,Kraftwerkszuordnung!$J$2:$J$52)</f>
+        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$37,B3,Kraftwerkszuordnung!$J$2:$J$37)</f>
         <v>34.4</v>
       </c>
       <c r="D3" s="3">
@@ -2905,7 +2247,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2913,8 +2255,8 @@
         <v>39</v>
       </c>
       <c r="C4" s="15">
-        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$52,B4,Kraftwerkszuordnung!$J$2:$J$52)</f>
-        <v>1753.3000000000002</v>
+        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$37,B4,Kraftwerkszuordnung!$J$2:$J$37)</f>
+        <v>698.15</v>
       </c>
       <c r="D4" s="3">
         <v>0.27</v>
@@ -2933,7 +2275,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2941,8 +2283,8 @@
         <v>17</v>
       </c>
       <c r="C5" s="15">
-        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$52,B5,Kraftwerkszuordnung!$J$2:$J$52)</f>
-        <v>3275.2000000000003</v>
+        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$37,B5,Kraftwerkszuordnung!$J$2:$J$37)</f>
+        <v>2380.75</v>
       </c>
       <c r="D5" s="3">
         <v>0.3</v>
@@ -2958,7 +2300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2966,8 +2308,8 @@
         <v>4</v>
       </c>
       <c r="C6" s="15">
-        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$52,B6,Kraftwerkszuordnung!$J$2:$J$52)</f>
-        <v>674.15</v>
+        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$37,B6,Kraftwerkszuordnung!$J$2:$J$37)</f>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
         <v>0.27</v>
@@ -2986,7 +2328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2994,7 +2336,7 @@
         <v>93</v>
       </c>
       <c r="C7" s="15">
-        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$52,B7,Kraftwerkszuordnung!$J$2:$J$52)</f>
+        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$37,B7,Kraftwerkszuordnung!$J$2:$J$37)</f>
         <v>10</v>
       </c>
       <c r="D7" s="3">
@@ -3011,7 +2353,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3019,8 +2361,8 @@
         <v>42</v>
       </c>
       <c r="C8" s="15">
-        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$52,B8,Kraftwerkszuordnung!$J$2:$J$52)</f>
-        <v>63.800000000000004</v>
+        <f>SUMIF(Kraftwerkszuordnung!$F$2:$F$37,B8,Kraftwerkszuordnung!$J$2:$J$37)</f>
+        <v>43.35</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -3034,18 +2376,18 @@
       <c r="G8" s="1"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
       <c r="C9" s="32"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="16">
         <f>SUM(C2:C9)</f>
-        <v>7496.05</v>
+        <v>3735.7</v>
       </c>
     </row>
   </sheetData>
@@ -3055,7 +2397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3063,7 +2405,7 @@
       <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -3074,7 +2416,7 @@
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -3103,7 +2445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>101</v>
       </c>
@@ -3131,7 +2473,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>102</v>
       </c>
@@ -3153,13 +2495,13 @@
       <c r="G3" s="8">
         <v>408.15</v>
       </c>
-      <c r="H3" s="1">
-        <f>Kraftwerkszuordnung!K3</f>
-        <v>122.44499999999999</v>
+      <c r="H3" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>103</v>
       </c>
@@ -3181,13 +2523,13 @@
       <c r="G4" s="8">
         <v>1055.1500000000001</v>
       </c>
-      <c r="H4" s="1">
-        <f>Kraftwerkszuordnung!K4</f>
-        <v>211.03</v>
+      <c r="H4" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>104</v>
       </c>
@@ -3210,12 +2552,12 @@
         <v>16.75</v>
       </c>
       <c r="H5" s="1">
-        <f>Kraftwerkszuordnung!K5</f>
+        <f>Kraftwerkszuordnung!K3</f>
         <v>0</v>
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>105</v>
       </c>
@@ -3237,13 +2579,13 @@
       <c r="G6" s="8">
         <v>808.15</v>
       </c>
-      <c r="H6" s="1">
-        <f>Kraftwerkszuordnung!K6</f>
-        <v>161.63</v>
+      <c r="H6" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>106</v>
       </c>
@@ -3265,13 +2607,13 @@
       <c r="G7" s="8">
         <v>75.150000000000006</v>
       </c>
-      <c r="H7" s="1">
-        <f>Kraftwerkszuordnung!K7</f>
-        <v>15.03</v>
+      <c r="H7" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>107</v>
       </c>
@@ -3294,12 +2636,12 @@
         <v>58.15</v>
       </c>
       <c r="H8" s="1">
-        <f>Kraftwerkszuordnung!K8</f>
+        <f>Kraftwerkszuordnung!K4</f>
         <v>11.63</v>
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>108</v>
       </c>
@@ -3322,12 +2664,12 @@
         <v>623.15</v>
       </c>
       <c r="H9" s="1">
-        <f>Kraftwerkszuordnung!K9</f>
+        <f>Kraftwerkszuordnung!K5</f>
         <v>186.94499999999999</v>
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>109</v>
       </c>
@@ -3350,12 +2692,12 @@
         <v>376.15</v>
       </c>
       <c r="H10" s="1">
-        <f>Kraftwerkszuordnung!K10</f>
+        <f>Kraftwerkszuordnung!K6</f>
         <v>112.845</v>
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>110</v>
       </c>
@@ -3378,12 +2720,12 @@
         <v>673.15</v>
       </c>
       <c r="H11" s="1">
-        <f>Kraftwerkszuordnung!K11</f>
+        <f>Kraftwerkszuordnung!K7</f>
         <v>201.94499999999999</v>
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>111</v>
       </c>
@@ -3405,13 +2747,13 @@
       <c r="G12" s="8">
         <v>36.15</v>
       </c>
-      <c r="H12" s="1">
-        <f>Kraftwerkszuordnung!K12</f>
-        <v>7.23</v>
+      <c r="H12" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>112</v>
       </c>
@@ -3433,13 +2775,13 @@
       <c r="G13" s="8">
         <v>131.15</v>
       </c>
-      <c r="H13" s="1">
-        <f>Kraftwerkszuordnung!K13</f>
-        <v>26.23</v>
+      <c r="H13" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>113</v>
       </c>
@@ -3461,13 +2803,13 @@
       <c r="G14" s="8">
         <v>3.15</v>
       </c>
-      <c r="H14" s="1">
-        <f>Kraftwerkszuordnung!K14</f>
-        <v>0</v>
+      <c r="H14" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>114</v>
       </c>
@@ -3490,12 +2832,12 @@
         <v>33.15</v>
       </c>
       <c r="H15" s="1">
-        <f>Kraftwerkszuordnung!K15</f>
+        <f>Kraftwerkszuordnung!K8</f>
         <v>0</v>
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>115</v>
       </c>
@@ -3517,461 +2859,461 @@
       <c r="G16" s="8">
         <v>9.85</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="17">
+        <v>150</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8">
+        <v>87.15</v>
+      </c>
+      <c r="H17" s="1">
+        <f>Kraftwerkszuordnung!K9</f>
+        <v>17.43</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17">
+        <v>380</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="8">
+        <v>674.15</v>
+      </c>
+      <c r="H18" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="17">
+        <v>150</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="8">
+        <v>13.85</v>
+      </c>
+      <c r="H19" s="1">
+        <f>Kraftwerkszuordnung!K10</f>
+        <v>2.77</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="17">
+        <v>150</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="H20" s="1">
+        <f>Kraftwerkszuordnung!K11</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="17">
+        <v>150</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="8">
+        <v>50.15</v>
+      </c>
+      <c r="H21" s="1">
+        <f>Kraftwerkszuordnung!K12</f>
+        <v>15.045</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="17">
+        <v>150</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8">
+        <v>3.15</v>
+      </c>
+      <c r="H22" s="1">
+        <f>Kraftwerkszuordnung!K13</f>
+        <v>0.63</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17">
+        <v>380</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="8">
+        <v>658.15</v>
+      </c>
+      <c r="H23" s="1">
+        <f>Kraftwerkszuordnung!K14</f>
+        <v>197.44499999999999</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="17">
+        <v>150</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="8">
+        <v>9.15</v>
+      </c>
+      <c r="H24" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="17">
+        <v>380</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="8">
+        <v>390.15</v>
+      </c>
+      <c r="H25" s="1">
+        <f>Kraftwerkszuordnung!K15</f>
+        <v>78.03</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="17">
+        <v>150</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="8">
+        <v>407.15</v>
+      </c>
+      <c r="H26" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="17">
+        <v>150</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="8">
+        <v>26.15</v>
+      </c>
+      <c r="H27" s="1">
         <f>Kraftwerkszuordnung!K16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D28" s="17">
+        <v>380</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="8">
+        <v>698.15</v>
+      </c>
+      <c r="H28" s="1">
+        <f>Kraftwerkszuordnung!K17</f>
+        <v>139.63</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="17">
         <v>150</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="8">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="H29" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="17">
+        <v>150</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="H30" s="1">
+        <f>Kraftwerkszuordnung!K18</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="17">
+        <v>150</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="8">
-        <v>87.15</v>
-      </c>
-      <c r="H17" s="1">
-        <f>Kraftwerkszuordnung!K17</f>
-        <v>17.43</v>
-      </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="17">
-        <v>380</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="8">
-        <v>674.15</v>
-      </c>
-      <c r="H18" s="1">
-        <f>Kraftwerkszuordnung!K18</f>
-        <v>134.83000000000001</v>
-      </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="17">
+      <c r="G31" s="8">
+        <v>10.15</v>
+      </c>
+      <c r="H31" s="1">
+        <f>Kraftwerkszuordnung!K19</f>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="17">
         <v>150</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="8">
-        <v>13.85</v>
-      </c>
-      <c r="H19" s="1">
-        <f>Kraftwerkszuordnung!K19</f>
-        <v>2.77</v>
-      </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="17">
-        <v>150</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="8">
-        <v>1.25</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="E32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="8">
+        <v>10</v>
+      </c>
+      <c r="H32" s="1">
         <f>Kraftwerkszuordnung!K20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="17">
-        <v>150</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="8">
-        <v>50.15</v>
-      </c>
-      <c r="H21" s="1">
-        <f>Kraftwerkszuordnung!K21</f>
-        <v>15.045</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="17">
-        <v>150</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="8">
-        <v>3.15</v>
-      </c>
-      <c r="H22" s="1">
-        <f>Kraftwerkszuordnung!K22</f>
-        <v>0.63</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="17">
-        <v>380</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="8">
-        <v>658.15</v>
-      </c>
-      <c r="H23" s="1">
-        <f>Kraftwerkszuordnung!K23</f>
-        <v>197.44499999999999</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="17">
-        <v>150</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="8">
-        <v>9.15</v>
-      </c>
-      <c r="H24" s="1">
-        <f>Kraftwerkszuordnung!K24</f>
-        <v>1.83</v>
-      </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="17">
-        <v>380</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="8">
-        <v>390.15</v>
-      </c>
-      <c r="H25" s="1">
-        <f>Kraftwerkszuordnung!K25</f>
-        <v>78.03</v>
-      </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="17">
-        <v>150</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="8">
-        <v>407.15</v>
-      </c>
-      <c r="H26" s="1">
-        <f>Kraftwerkszuordnung!K26</f>
-        <v>122.145</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="17">
-        <v>150</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="8">
-        <v>26.15</v>
-      </c>
-      <c r="H27" s="1">
-        <f>Kraftwerkszuordnung!K27</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="17">
-        <v>380</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="8">
-        <v>698.15</v>
-      </c>
-      <c r="H28" s="1">
-        <f>Kraftwerkszuordnung!K28</f>
-        <v>139.63</v>
-      </c>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="17">
-        <v>150</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="8">
-        <v>79.150000000000006</v>
-      </c>
-      <c r="H29" s="1">
-        <f>Kraftwerkszuordnung!K29</f>
-        <v>23.745000000000001</v>
-      </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="17">
-        <v>150</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="8">
-        <v>0.45</v>
-      </c>
-      <c r="H30" s="1">
-        <f>Kraftwerkszuordnung!K30</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="17">
-        <v>150</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" s="8">
-        <v>10.15</v>
-      </c>
-      <c r="H31" s="1">
-        <f>Kraftwerkszuordnung!K31</f>
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="17">
-        <v>150</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G32" s="8">
-        <v>10</v>
-      </c>
-      <c r="H32" s="1">
-        <f>Kraftwerkszuordnung!K32</f>
-        <v>0</v>
-      </c>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>132</v>
       </c>
@@ -3993,13 +3335,13 @@
       <c r="G33" s="8">
         <v>55.15</v>
       </c>
-      <c r="H33" s="1">
-        <f>Kraftwerkszuordnung!K33</f>
-        <v>11.03</v>
+      <c r="H33" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>133</v>
       </c>
@@ -4022,12 +3364,12 @@
         <v>1.75</v>
       </c>
       <c r="H34" s="1">
-        <f>Kraftwerkszuordnung!K34</f>
+        <f>Kraftwerkszuordnung!K21</f>
         <v>0.35</v>
       </c>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>134</v>
       </c>
@@ -4050,12 +3392,12 @@
         <v>2.85</v>
       </c>
       <c r="H35" s="1">
-        <f>Kraftwerkszuordnung!K35</f>
+        <f>Kraftwerkszuordnung!K22</f>
         <v>0.56999999999999995</v>
       </c>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>135</v>
       </c>
@@ -4077,13 +3419,13 @@
       <c r="G36" s="8">
         <v>1.25</v>
       </c>
-      <c r="H36" s="1">
-        <f>Kraftwerkszuordnung!K36</f>
-        <v>0.25</v>
+      <c r="H36" s="1" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>136</v>
       </c>
@@ -4105,13 +3447,13 @@
       <c r="G37" s="8">
         <v>7.45</v>
       </c>
-      <c r="H37" s="21">
-        <f>Kraftwerkszuordnung!K37</f>
-        <v>0</v>
+      <c r="H37" s="21" t="e">
+        <f>Kraftwerkszuordnung!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="I37" s="18"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="29"/>
       <c r="C38" s="28"/>
@@ -4122,7 +3464,7 @@
       <c r="H38" s="12"/>
       <c r="I38" s="28"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="22"/>
       <c r="C39" s="27"/>
@@ -4133,7 +3475,7 @@
       <c r="H39" s="26"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="22"/>
       <c r="C40" s="4"/>
@@ -4144,7 +3486,7 @@
       <c r="H40" s="26"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="22"/>
       <c r="C41" s="4"/>
@@ -4155,7 +3497,7 @@
       <c r="H41" s="26"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="22"/>
       <c r="C42" s="4"/>
@@ -4166,7 +3508,7 @@
       <c r="H42" s="26"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="22"/>
       <c r="C43" s="4"/>
@@ -4177,7 +3519,7 @@
       <c r="H43" s="26"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="22"/>
       <c r="C44" s="4"/>
@@ -4188,7 +3530,7 @@
       <c r="H44" s="26"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="22"/>
       <c r="C45" s="27"/>
@@ -4199,7 +3541,7 @@
       <c r="H45" s="26"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="22"/>
       <c r="C46" s="4"/>
@@ -4210,7 +3552,7 @@
       <c r="H46" s="26"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="22"/>
       <c r="C47" s="23"/>
@@ -4221,7 +3563,7 @@
       <c r="H47" s="26"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="22"/>
       <c r="C48" s="23"/>
@@ -4232,7 +3574,7 @@
       <c r="H48" s="26"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="22"/>
       <c r="C49" s="4"/>
@@ -4243,7 +3585,7 @@
       <c r="H49" s="26"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="22"/>
       <c r="C50" s="4"/>
@@ -4254,7 +3596,7 @@
       <c r="H50" s="26"/>
       <c r="I50" s="4"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="22"/>
       <c r="C51" s="4"/>
@@ -4265,7 +3607,7 @@
       <c r="H51" s="26"/>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="22"/>
       <c r="C52" s="4"/>
@@ -4276,21 +3618,21 @@
       <c r="H52" s="26"/>
       <c r="I52" s="4"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
@@ -4301,7 +3643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4309,7 +3651,7 @@
       <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
@@ -4319,12 +3661,12 @@
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
@@ -4350,7 +3692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -4368,7 +3710,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -4397,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -4426,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -4455,7 +3797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
@@ -4484,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
@@ -4513,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -4542,7 +3884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>47</v>
       </c>
@@ -4571,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -4600,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
@@ -4629,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -4658,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -4687,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
@@ -4716,7 +4058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>59</v>
       </c>
@@ -4745,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
@@ -4774,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>63</v>
       </c>
@@ -4803,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>65</v>
       </c>
@@ -4832,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>66</v>
       </c>
@@ -4861,7 +4203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>68</v>
       </c>
@@ -4890,7 +4232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>70</v>
       </c>
@@ -4919,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>72</v>
       </c>
@@ -4948,7 +4290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
@@ -4977,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>76</v>
       </c>
@@ -5006,7 +4348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>78</v>
       </c>
@@ -5035,7 +4377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>79</v>
       </c>
@@ -5064,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>80</v>
       </c>
@@ -5093,7 +4435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>82</v>
       </c>
@@ -5122,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
@@ -5151,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>86</v>
       </c>
@@ -5180,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
@@ -5209,7 +4551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
@@ -5238,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
@@ -5267,7 +4609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>96</v>
       </c>
@@ -5296,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>99</v>
       </c>
@@ -5325,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>137</v>
       </c>
@@ -5361,14 +4703,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AL38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -5386,7 +4728,7 @@
     <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38">
+    <row r="1" spans="2:38" x14ac:dyDescent="0.25">
       <c r="C1" s="38" t="s">
         <v>12</v>
       </c>
@@ -5496,7 +4838,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="2:38">
+    <row r="2" spans="2:38" x14ac:dyDescent="0.25">
       <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
@@ -5606,7 +4948,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="2:38">
+    <row r="3" spans="2:38" x14ac:dyDescent="0.25">
       <c r="C3" s="38" t="s">
         <v>143</v>
       </c>
@@ -5716,12 +5058,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:38">
+    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:38">
+    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
@@ -5774,7 +5116,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:38">
+    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
@@ -5923,7 +5265,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:38">
+    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
@@ -6072,7 +5414,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:38">
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
@@ -6221,7 +5563,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:38">
+    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
@@ -6370,7 +5712,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:38">
+    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
@@ -6519,7 +5861,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:38">
+    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>47</v>
       </c>
@@ -6668,7 +6010,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:38">
+    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
@@ -6817,7 +6159,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:38">
+    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>51</v>
       </c>
@@ -6966,7 +6308,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:38">
+    <row r="14" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>53</v>
       </c>
@@ -7115,7 +6457,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:38">
+    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>55</v>
       </c>
@@ -7264,7 +6606,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:38">
+    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
@@ -7413,7 +6755,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:38">
+    <row r="17" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
@@ -7562,7 +6904,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:38">
+    <row r="18" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>60</v>
       </c>
@@ -7711,7 +7053,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:38">
+    <row r="19" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>63</v>
       </c>
@@ -7860,7 +7202,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:38">
+    <row r="20" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
@@ -8009,7 +7351,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:38">
+    <row r="21" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>66</v>
       </c>
@@ -8158,7 +7500,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:38">
+    <row r="22" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>68</v>
       </c>
@@ -8307,7 +7649,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:38">
+    <row r="23" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>70</v>
       </c>
@@ -8456,7 +7798,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:38">
+    <row r="24" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>72</v>
       </c>
@@ -8605,7 +7947,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:38">
+    <row r="25" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>74</v>
       </c>
@@ -8754,7 +8096,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:38">
+    <row r="26" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>76</v>
       </c>
@@ -8903,7 +8245,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:38">
+    <row r="27" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>78</v>
       </c>
@@ -9052,7 +8394,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:38">
+    <row r="28" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>79</v>
       </c>
@@ -9201,7 +8543,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:38">
+    <row r="29" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
@@ -9350,7 +8692,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:38">
+    <row r="30" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>82</v>
       </c>
@@ -9499,7 +8841,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:38">
+    <row r="31" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>84</v>
       </c>
@@ -9648,7 +8990,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:38">
+    <row r="32" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>86</v>
       </c>
@@ -9797,7 +9139,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:38">
+    <row r="33" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>88</v>
       </c>
@@ -9946,7 +9288,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:38">
+    <row r="34" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>90</v>
       </c>
@@ -10095,7 +9437,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:38">
+    <row r="35" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>94</v>
       </c>
@@ -10244,7 +9586,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:38">
+    <row r="36" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>96</v>
       </c>
@@ -10393,7 +9735,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:38">
+    <row r="37" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B37" s="18" t="s">
         <v>99</v>
       </c>
@@ -10542,7 +9884,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:38">
+    <row r="38" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>137</v>
       </c>
@@ -10697,7 +10039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -10705,7 +10047,7 @@
       <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.85546875" customWidth="1"/>
@@ -10715,12 +10057,12 @@
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
@@ -10746,7 +10088,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -10764,7 +10106,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>90</v>
       </c>
@@ -10793,7 +10135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
@@ -10803,18 +10145,18 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" s="6"/>
     </row>
   </sheetData>
@@ -10824,16 +10166,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1" s="38" t="s">
         <v>12</v>
       </c>
@@ -10841,7 +10183,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
@@ -10849,7 +10191,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="38" t="s">
         <v>143</v>
       </c>
@@ -10857,12 +10199,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>90</v>
       </c>

</xml_diff>